<commit_message>
Put stage names back that were mistakenly deleted
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/data/Lincoln2023.xlsx
+++ b/Tests/Validation/Wheat/data/Lincoln2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\ApsimX\Tests\Validation\Wheat\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC41435-8CD9-4819-B731-8D442CD9AEDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747C948F-E69B-4C58-A9B2-8B891DEDB0AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3769" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3839" uniqueCount="93">
   <si>
     <t>SimulationName</t>
   </si>
@@ -306,6 +306,21 @@
   </si>
   <si>
     <t>Wheat.Phenology.Zadok.Stage-NotModeled</t>
+  </si>
+  <si>
+    <t>FlafLeaf</t>
+  </si>
+  <si>
+    <t>GrainFilling</t>
+  </si>
+  <si>
+    <t>HarvestRipe</t>
+  </si>
+  <si>
+    <t>2ndNodeOnMainStem</t>
+  </si>
+  <si>
+    <t>EndGrainFill</t>
   </si>
 </sst>
 </file>
@@ -62629,11 +62644,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE1866"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="6" topLeftCell="R109" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomRight" activeCell="U7" sqref="U7:V126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -62972,6 +62987,12 @@
       <c r="S7">
         <v>9.1671242849999999</v>
       </c>
+      <c r="U7">
+        <v>39</v>
+      </c>
+      <c r="V7" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -63010,6 +63031,12 @@
       <c r="S8">
         <v>6.9917530110000001</v>
       </c>
+      <c r="U8">
+        <v>60</v>
+      </c>
+      <c r="V8" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -63048,6 +63075,12 @@
       <c r="S9">
         <v>3.031436002</v>
       </c>
+      <c r="U9">
+        <v>79</v>
+      </c>
+      <c r="V9" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -63098,6 +63131,12 @@
       <c r="P10">
         <v>4.5335116000000002E-2</v>
       </c>
+      <c r="U10">
+        <v>90</v>
+      </c>
+      <c r="V10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -63327,7 +63366,7 @@
         <v>8.2800065689999993</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -63364,8 +63403,14 @@
       <c r="S17">
         <v>7.805443007</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U17">
+        <v>39</v>
+      </c>
+      <c r="V17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -63402,8 +63447,14 @@
       <c r="S18">
         <v>6.4326701570000004</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U18">
+        <v>60</v>
+      </c>
+      <c r="V18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -63440,8 +63491,14 @@
       <c r="S19">
         <v>1.8282202089999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U19">
+        <v>79</v>
+      </c>
+      <c r="V19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -63490,8 +63547,14 @@
       <c r="P20">
         <v>4.2786942000000001E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U20">
+        <v>90</v>
+      </c>
+      <c r="V20" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -63529,7 +63592,7 @@
         <v>0.111784605</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -63567,7 +63630,7 @@
         <v>0.99788239199999995</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -63604,8 +63667,14 @@
       <c r="S23">
         <v>3.1507037260000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U23">
+        <v>30</v>
+      </c>
+      <c r="V23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -63642,8 +63711,14 @@
       <c r="S24">
         <v>5.4600551260000003</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U24">
+        <v>32</v>
+      </c>
+      <c r="V24" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -63680,8 +63755,14 @@
       <c r="S25">
         <v>8.6491989730000007</v>
       </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U25">
+        <v>39</v>
+      </c>
+      <c r="V25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -63718,8 +63799,14 @@
       <c r="S26">
         <v>7.5838782550000001</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U26">
+        <v>60</v>
+      </c>
+      <c r="V26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -63756,8 +63843,14 @@
       <c r="S27">
         <v>3.944227277</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U27">
+        <v>79</v>
+      </c>
+      <c r="V27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -63806,8 +63899,14 @@
       <c r="P28">
         <v>3.9290705000000002E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U28">
+        <v>90</v>
+      </c>
+      <c r="V28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -63845,7 +63944,7 @@
         <v>0.17846519899999999</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -63883,7 +63982,7 @@
         <v>1.1048471230000001</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -63921,7 +64020,7 @@
         <v>2.2666835289999998</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -63959,7 +64058,7 @@
         <v>4.2972114469999996</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>28</v>
       </c>
@@ -63997,7 +64096,7 @@
         <v>5.5627188219999999</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -64034,8 +64133,14 @@
       <c r="S34">
         <v>8.5318740389999999</v>
       </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U34">
+        <v>39</v>
+      </c>
+      <c r="V34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>28</v>
       </c>
@@ -64072,8 +64177,14 @@
       <c r="S35">
         <v>7.8088340599999997</v>
       </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U35">
+        <v>60</v>
+      </c>
+      <c r="V35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>28</v>
       </c>
@@ -64110,8 +64221,14 @@
       <c r="S36">
         <v>4.1330800160000001</v>
       </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U36">
+        <v>79</v>
+      </c>
+      <c r="V36" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>28</v>
       </c>
@@ -64160,8 +64277,14 @@
       <c r="P37">
         <v>4.1537956000000001E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U37">
+        <v>90</v>
+      </c>
+      <c r="V37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>29</v>
       </c>
@@ -64199,7 +64322,7 @@
         <v>0.30112680600000002</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>29</v>
       </c>
@@ -64237,7 +64360,7 @@
         <v>1.551725281</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>29</v>
       </c>
@@ -64275,7 +64398,7 @@
         <v>2.114635952</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>29</v>
       </c>
@@ -64313,7 +64436,7 @@
         <v>2.3638819400000002</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>29</v>
       </c>
@@ -64350,8 +64473,14 @@
       <c r="S42">
         <v>4.747518693</v>
       </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U42">
+        <v>32</v>
+      </c>
+      <c r="V42" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>29</v>
       </c>
@@ -64389,7 +64518,7 @@
         <v>8.4090034350000007</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>29</v>
       </c>
@@ -64426,8 +64555,14 @@
       <c r="S44">
         <v>8.7706887820000006</v>
       </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U44">
+        <v>39</v>
+      </c>
+      <c r="V44" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>29</v>
       </c>
@@ -64464,8 +64599,14 @@
       <c r="S45">
         <v>6.7804361369999997</v>
       </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U45">
+        <v>60</v>
+      </c>
+      <c r="V45" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>29</v>
       </c>
@@ -64502,8 +64643,14 @@
       <c r="S46">
         <v>2.8845222499999998</v>
       </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U46">
+        <v>79</v>
+      </c>
+      <c r="V46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>29</v>
       </c>
@@ -64552,8 +64699,14 @@
       <c r="P47">
         <v>4.1070628999999997E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U47">
+        <v>90</v>
+      </c>
+      <c r="V47" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>30</v>
       </c>
@@ -64591,7 +64744,7 @@
         <v>9.5170099999999994E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>30</v>
       </c>
@@ -64629,7 +64782,7 @@
         <v>0.832403228</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>30</v>
       </c>
@@ -64666,8 +64819,14 @@
       <c r="S50">
         <v>2.5001918129999998</v>
       </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U50">
+        <v>30</v>
+      </c>
+      <c r="V50" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>30</v>
       </c>
@@ -64704,8 +64863,14 @@
       <c r="S51">
         <v>4.7929767810000001</v>
       </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U51">
+        <v>32</v>
+      </c>
+      <c r="V51" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>30</v>
       </c>
@@ -64742,8 +64907,14 @@
       <c r="S52">
         <v>7.9932928780000001</v>
       </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U52">
+        <v>39</v>
+      </c>
+      <c r="V52" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>30</v>
       </c>
@@ -64780,8 +64951,14 @@
       <c r="S53">
         <v>7.6577684540000002</v>
       </c>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U53">
+        <v>60</v>
+      </c>
+      <c r="V53" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>30</v>
       </c>
@@ -64818,8 +64995,14 @@
       <c r="S54">
         <v>4.226584849</v>
       </c>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U54">
+        <v>79</v>
+      </c>
+      <c r="V54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>30</v>
       </c>
@@ -64868,8 +65051,14 @@
       <c r="P55">
         <v>3.6213024000000003E-2</v>
       </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U55">
+        <v>90</v>
+      </c>
+      <c r="V55" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>31</v>
       </c>
@@ -64907,7 +65096,7 @@
         <v>0.41784933600000002</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>31</v>
       </c>
@@ -64945,7 +65134,7 @@
         <v>1.986494494</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>31</v>
       </c>
@@ -64983,7 +65172,7 @@
         <v>3.6943126030000002</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>31</v>
       </c>
@@ -65021,7 +65210,7 @@
         <v>5.3521747299999998</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>31</v>
       </c>
@@ -65059,7 +65248,7 @@
         <v>4.9286069960000001</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>31</v>
       </c>
@@ -65097,7 +65286,7 @@
         <v>5.8044072489999996</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>31</v>
       </c>
@@ -65134,8 +65323,14 @@
       <c r="S62">
         <v>8.0077171759999999</v>
       </c>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U62">
+        <v>39</v>
+      </c>
+      <c r="V62" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>31</v>
       </c>
@@ -65172,8 +65367,14 @@
       <c r="S63">
         <v>6.290248697</v>
       </c>
-    </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U63">
+        <v>60</v>
+      </c>
+      <c r="V63" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>31</v>
       </c>
@@ -65210,8 +65411,14 @@
       <c r="S64">
         <v>3.1669385889999999</v>
       </c>
-    </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U64">
+        <v>79</v>
+      </c>
+      <c r="V64" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>31</v>
       </c>
@@ -65260,8 +65467,14 @@
       <c r="P65">
         <v>4.4811206999999999E-2</v>
       </c>
-    </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U65">
+        <v>90</v>
+      </c>
+      <c r="V65" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>32</v>
       </c>
@@ -65299,7 +65512,7 @@
         <v>0.55831055100000004</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>32</v>
       </c>
@@ -65337,7 +65550,7 @@
         <v>2.3448339539999998</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>32</v>
       </c>
@@ -65375,7 +65588,7 @@
         <v>3.3576053610000001</v>
       </c>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>32</v>
       </c>
@@ -65413,7 +65626,7 @@
         <v>3.3483505729999998</v>
       </c>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>32</v>
       </c>
@@ -65450,8 +65663,14 @@
       <c r="S70">
         <v>5.2360987879999996</v>
       </c>
-    </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U70">
+        <v>32</v>
+      </c>
+      <c r="V70" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>32</v>
       </c>
@@ -65488,8 +65707,14 @@
       <c r="S71">
         <v>7.8778786040000002</v>
       </c>
-    </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U71">
+        <v>39</v>
+      </c>
+      <c r="V71" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>32</v>
       </c>
@@ -65526,8 +65751,14 @@
       <c r="S72">
         <v>6.9580777070000002</v>
       </c>
-    </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U72">
+        <v>60</v>
+      </c>
+      <c r="V72" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>32</v>
       </c>
@@ -65564,8 +65795,14 @@
       <c r="S73">
         <v>4.6551906570000003</v>
       </c>
-    </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U73">
+        <v>79</v>
+      </c>
+      <c r="V73" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>32</v>
       </c>
@@ -65614,8 +65851,14 @@
       <c r="P74">
         <v>4.3455645000000001E-2</v>
       </c>
-    </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U74">
+        <v>90</v>
+      </c>
+      <c r="V74" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>33</v>
       </c>
@@ -65653,7 +65896,7 @@
         <v>0.13447837100000001</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>33</v>
       </c>
@@ -65691,7 +65934,7 @@
         <v>1.06995061</v>
       </c>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>33</v>
       </c>
@@ -65728,8 +65971,14 @@
       <c r="S77">
         <v>2.7417977100000002</v>
       </c>
-    </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U77">
+        <v>30</v>
+      </c>
+      <c r="V77" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>33</v>
       </c>
@@ -65766,8 +66015,14 @@
       <c r="S78">
         <v>4.4151943400000002</v>
       </c>
-    </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U78">
+        <v>32</v>
+      </c>
+      <c r="V78" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>33</v>
       </c>
@@ -65804,8 +66059,14 @@
       <c r="S79">
         <v>6.6267833469999999</v>
       </c>
-    </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U79">
+        <v>39</v>
+      </c>
+      <c r="V79" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>33</v>
       </c>
@@ -65842,8 +66103,14 @@
       <c r="S80">
         <v>6.9780389630000004</v>
       </c>
-    </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U80">
+        <v>60</v>
+      </c>
+      <c r="V80" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="81" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>33</v>
       </c>
@@ -65880,8 +66147,14 @@
       <c r="S81">
         <v>4.8895358199999999</v>
       </c>
-    </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U81">
+        <v>79</v>
+      </c>
+      <c r="V81" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="82" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>33</v>
       </c>
@@ -65930,8 +66203,14 @@
       <c r="P82">
         <v>4.4440269999999997E-2</v>
       </c>
-    </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U82">
+        <v>90</v>
+      </c>
+      <c r="V82" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="83" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>34</v>
       </c>
@@ -65969,7 +66248,7 @@
         <v>0.298632383</v>
       </c>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>34</v>
       </c>
@@ -66007,7 +66286,7 @@
         <v>1.5364923539999999</v>
       </c>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>34</v>
       </c>
@@ -66045,7 +66324,7 @@
         <v>3.5987345730000002</v>
       </c>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>34</v>
       </c>
@@ -66083,7 +66362,7 @@
         <v>4.2978236699999997</v>
       </c>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>34</v>
       </c>
@@ -66121,7 +66400,7 @@
         <v>5.7396719359999997</v>
       </c>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>34</v>
       </c>
@@ -66159,7 +66438,7 @@
         <v>5.2155868720000003</v>
       </c>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>34</v>
       </c>
@@ -66196,8 +66475,14 @@
       <c r="S89">
         <v>8.7662585289999999</v>
       </c>
-    </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U89">
+        <v>39</v>
+      </c>
+      <c r="V89" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="90" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>34</v>
       </c>
@@ -66234,8 +66519,14 @@
       <c r="S90">
         <v>6.9086497590000002</v>
       </c>
-    </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U90">
+        <v>60</v>
+      </c>
+      <c r="V90" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="91" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>34</v>
       </c>
@@ -66272,8 +66563,14 @@
       <c r="S91">
         <v>3.903384601</v>
       </c>
-    </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U91">
+        <v>79</v>
+      </c>
+      <c r="V91" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="92" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>34</v>
       </c>
@@ -66322,8 +66619,14 @@
       <c r="P92">
         <v>4.4291780000000003E-2</v>
       </c>
-    </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U92">
+        <v>90</v>
+      </c>
+      <c r="V92" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>35</v>
       </c>
@@ -66361,7 +66664,7 @@
         <v>0.42581798599999998</v>
       </c>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>35</v>
       </c>
@@ -66399,7 +66702,7 @@
         <v>2.300822675</v>
       </c>
     </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>35</v>
       </c>
@@ -66437,7 +66740,7 @@
         <v>2.9564560110000002</v>
       </c>
     </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>35</v>
       </c>
@@ -66475,7 +66778,7 @@
         <v>2.6335862529999998</v>
       </c>
     </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>35</v>
       </c>
@@ -66513,7 +66816,7 @@
         <v>4.5004497480000003</v>
       </c>
     </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>35</v>
       </c>
@@ -66551,7 +66854,7 @@
         <v>8.7208325640000002</v>
       </c>
     </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>35</v>
       </c>
@@ -66588,8 +66891,14 @@
       <c r="S99">
         <v>8.1373795520000005</v>
       </c>
-    </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U99">
+        <v>39</v>
+      </c>
+      <c r="V99" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="100" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>35</v>
       </c>
@@ -66626,8 +66935,14 @@
       <c r="S100">
         <v>7.0123124219999999</v>
       </c>
-    </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U100">
+        <v>60</v>
+      </c>
+      <c r="V100" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="101" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>35</v>
       </c>
@@ -66664,8 +66979,14 @@
       <c r="S101">
         <v>3.292981884</v>
       </c>
-    </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U101">
+        <v>79</v>
+      </c>
+      <c r="V101" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="102" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>35</v>
       </c>
@@ -66714,8 +67035,14 @@
       <c r="P102">
         <v>4.2917726000000003E-2</v>
       </c>
-    </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U102">
+        <v>90</v>
+      </c>
+      <c r="V102" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="103" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>36</v>
       </c>
@@ -66753,7 +67080,7 @@
         <v>0.126097761</v>
       </c>
     </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>36</v>
       </c>
@@ -66791,7 +67118,7 @@
         <v>0.97963529500000002</v>
       </c>
     </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>36</v>
       </c>
@@ -66828,8 +67155,14 @@
       <c r="S105">
         <v>2.6580066819999999</v>
       </c>
-    </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U105">
+        <v>30</v>
+      </c>
+      <c r="V105" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="106" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>36</v>
       </c>
@@ -66866,8 +67199,14 @@
       <c r="S106">
         <v>5.0239455939999997</v>
       </c>
-    </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U106">
+        <v>32</v>
+      </c>
+      <c r="V106" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="107" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>36</v>
       </c>
@@ -66904,8 +67243,14 @@
       <c r="S107">
         <v>7.952495077</v>
       </c>
-    </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U107">
+        <v>39</v>
+      </c>
+      <c r="V107" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="108" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>36</v>
       </c>
@@ -66942,8 +67287,14 @@
       <c r="S108">
         <v>7.2405623859999997</v>
       </c>
-    </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U108">
+        <v>60</v>
+      </c>
+      <c r="V108" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="109" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>36</v>
       </c>
@@ -66980,8 +67331,14 @@
       <c r="S109">
         <v>3.9712046430000001</v>
       </c>
-    </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U109">
+        <v>79</v>
+      </c>
+      <c r="V109" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="110" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>36</v>
       </c>
@@ -67030,8 +67387,14 @@
       <c r="P110">
         <v>3.6001126000000001E-2</v>
       </c>
-    </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U110">
+        <v>90</v>
+      </c>
+      <c r="V110" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="111" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>37</v>
       </c>
@@ -67069,7 +67432,7 @@
         <v>0.11363327199999999</v>
       </c>
     </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>37</v>
       </c>
@@ -67144,6 +67507,12 @@
       <c r="S113">
         <v>4.0657695010000001</v>
       </c>
+      <c r="U113">
+        <v>30</v>
+      </c>
+      <c r="V113" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="114" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
@@ -67182,6 +67551,12 @@
       <c r="S114">
         <v>3.8710286620000001</v>
       </c>
+      <c r="U114">
+        <v>32</v>
+      </c>
+      <c r="V114" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="115" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
@@ -67220,6 +67595,12 @@
       <c r="S115">
         <v>9.0441546759999998</v>
       </c>
+      <c r="U115">
+        <v>39</v>
+      </c>
+      <c r="V115" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="116" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
@@ -67258,6 +67639,12 @@
       <c r="S116">
         <v>7.5074018699999998</v>
       </c>
+      <c r="U116">
+        <v>60</v>
+      </c>
+      <c r="V116" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="117" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
@@ -67296,6 +67683,12 @@
       <c r="S117">
         <v>4.751518785</v>
       </c>
+      <c r="U117">
+        <v>79</v>
+      </c>
+      <c r="V117" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="118" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
@@ -67346,6 +67739,12 @@
       <c r="P118">
         <v>3.7851594000000002E-2</v>
       </c>
+      <c r="U118">
+        <v>90</v>
+      </c>
+      <c r="V118" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="119" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
@@ -67460,6 +67859,12 @@
       <c r="S121">
         <v>2.598802777</v>
       </c>
+      <c r="U121">
+        <v>30</v>
+      </c>
+      <c r="V121" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="122" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
@@ -67498,6 +67903,12 @@
       <c r="S122">
         <v>4.0273256340000003</v>
       </c>
+      <c r="U122">
+        <v>32</v>
+      </c>
+      <c r="V122" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="123" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
@@ -67536,6 +67947,12 @@
       <c r="S123">
         <v>7.0854080960000001</v>
       </c>
+      <c r="U123">
+        <v>39</v>
+      </c>
+      <c r="V123" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="124" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
@@ -67574,6 +67991,12 @@
       <c r="S124">
         <v>5.9431640489999999</v>
       </c>
+      <c r="U124">
+        <v>60</v>
+      </c>
+      <c r="V124" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="125" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
@@ -67612,6 +68035,12 @@
       <c r="S125">
         <v>3.911031666</v>
       </c>
+      <c r="U125">
+        <v>79</v>
+      </c>
+      <c r="V125" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="126" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
@@ -67661,6 +68090,12 @@
       </c>
       <c r="P126">
         <v>3.5139576999999998E-2</v>
+      </c>
+      <c r="U126">
+        <v>90</v>
+      </c>
+      <c r="V126" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="127" spans="1:23" x14ac:dyDescent="0.25">
@@ -94480,7 +94915,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D3A1DD-6556-4C13-9BED-B6412B226627}">
   <dimension ref="A3:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A20" sqref="A20:F34"/>
     </sheetView>
   </sheetViews>

</xml_diff>